<commit_message>
updated risks are a result of team meeting 9/23
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C33062
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY3_eCoaching Log Risk Register.xlsx
+++ b/Project Management/CCO OY3_eCoaching Log Risk Register.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="97">
   <si>
     <t>Status</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>no email sent</t>
+  </si>
+  <si>
+    <t>Closed row 13</t>
   </si>
 </sst>
 </file>
@@ -1530,8 +1533,8 @@
   </sheetPr>
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,7 +1806,7 @@
       </c>
       <c r="V5" s="7"/>
     </row>
-    <row r="6" spans="1:22" ht="82.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
@@ -2243,7 +2246,7 @@
     </row>
     <row r="13" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="4" t="s">
@@ -2252,7 +2255,9 @@
       <c r="D13" s="9">
         <v>42137</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="9">
+        <v>42270</v>
+      </c>
       <c r="F13" s="5" t="s">
         <v>84</v>
       </c>
@@ -3259,10 +3264,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3300,6 +3305,14 @@
       </c>
       <c r="B4" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>42270</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3314,6 +3327,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E5C6E04F5F2CA4DBF07DC2DA055DA5A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b67af60ff7fc8b8e5184fdb460baaf96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -3427,31 +3449,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9FB9A1-B4D8-4EF0-9C41-8E101BF6B1F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3465,12 +3486,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update risk for Feb 2016
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C33757
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY3_eCoaching Log Risk Register.xlsx
+++ b/Project Management/CCO OY3_eCoaching Log Risk Register.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="107">
   <si>
     <t>Status</t>
   </si>
@@ -93,10 +93,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Total Impact on occurance
-$</t>
-  </si>
-  <si>
     <t>Risk Exposure Ranking
 (1 - 25)</t>
   </si>
@@ -137,9 +133,6 @@
     <t>Provide training for users. Ensure that the message is reinforced through coaching. Provide SOPs for users</t>
   </si>
   <si>
-    <t>Incomplete and inaccurate data in centrallized CCO CSR/Employee database</t>
-  </si>
-  <si>
     <t>Utilizing LimeSurvey and Verint; new scorecard and scoring system</t>
   </si>
   <si>
@@ -198,9 +191,6 @@
   </si>
   <si>
     <t>Risk is closed</t>
-  </si>
-  <si>
-    <t>Lack of hierarchy information - supervisor--&gt; manager--&gt; sr. manager in peoplesoft feed</t>
   </si>
   <si>
     <t>Suzy</t>
@@ -231,27 +221,15 @@
     <t>Balance work load across engineers to the greatest extent possible to prevent distractions.</t>
   </si>
   <si>
-    <t>Closed 2/23/15 - hierarchy information is in the peoplesoft file</t>
-  </si>
-  <si>
     <t>Date Modified</t>
   </si>
   <si>
-    <t>Resources are supporting eCL, Performance Scorecard, A&amp;E, IQS</t>
-  </si>
-  <si>
     <t>Monitoring system changes; Verint went into production July 1, 2014; closed 2/23/15</t>
   </si>
   <si>
-    <t>new</t>
-  </si>
-  <si>
     <t>closed</t>
   </si>
   <si>
-    <t>Incomplete and inaccurate data in centralized CCO CSR/Employee database (eWFM/roster raw) - creates inconsistencies in records being created from external sources (quality control system) compared to records created directly in eCL.</t>
-  </si>
-  <si>
     <t>access to warning information</t>
   </si>
   <si>
@@ -270,9 +248,6 @@
     <t>Exposure</t>
   </si>
   <si>
-    <t>individuals identified in OY3 will be more aligned with the project</t>
-  </si>
-  <si>
     <t>added risk on warnings</t>
   </si>
   <si>
@@ -291,9 +266,6 @@
     <t>Open</t>
   </si>
   <si>
-    <t>File share access changing without warning</t>
-  </si>
-  <si>
     <t>Application will not work</t>
   </si>
   <si>
@@ -303,9 +275,6 @@
     <t>Program: CCO OY3 eCoaching Log Risk Register</t>
   </si>
   <si>
-    <t>Queen</t>
-  </si>
-  <si>
     <t>Jourdain</t>
   </si>
   <si>
@@ -322,6 +291,67 @@
   </si>
   <si>
     <t>Closed row 13</t>
+  </si>
+  <si>
+    <t>Incomplete and inaccurate data in centralized CCO CSR/Employee database (eWFM/People Soft) - creates inconsistencies in records being created from external sources (quality control system) compared to records created directly in eCL.</t>
+  </si>
+  <si>
+    <t>Resources are supporting other engineering projects</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>File share access changing without warning. This occurred on 1/16/2016</t>
+  </si>
+  <si>
+    <t>individuals identified in OY3/OY4 will be more aligned with the project</t>
+  </si>
+  <si>
+    <t>work being delayed</t>
+  </si>
+  <si>
+    <t>Rely on HR to make HR Job Code updates in their system.  We are low priority for them</t>
+  </si>
+  <si>
+    <t>HR Job Code change dependences in the eCL system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job Code changes are not communicated and the eCL system requires modifications to function properly </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> delay of feed updates impact our delivery time for eCL system updates</t>
+  </si>
+  <si>
+    <t>Total Impact on occurrence
+$</t>
+  </si>
+  <si>
+    <t>Incomplete and inaccurate data in centralized CCO CSR/Employee database</t>
+  </si>
+  <si>
+    <t>Lack of hierarchy information - supervisor--&gt; manager--&gt; sr. manager in PeopleSoft feed</t>
+  </si>
+  <si>
+    <t>Closed 2/23/15 - hierarchy information is in the PeopleSoft file</t>
+  </si>
+  <si>
+    <t>Work with HR to have them communicate Job Code change to us in advance so we have additional time to make eCL system changes</t>
+  </si>
+  <si>
+    <t>Job Code change notifications</t>
+  </si>
+  <si>
+    <t>setup manual entry</t>
+  </si>
+  <si>
+    <t>Work with HR to have them make changes in a more timely manor</t>
+  </si>
+  <si>
+    <t>manual activate them in eCL system</t>
+  </si>
+  <si>
+    <t>Updated in accurate data, engineering resource risk and file share risks.  Added 2 new risks related to Job Code changes</t>
   </si>
 </sst>
 </file>
@@ -1223,10 +1253,10 @@
     <tableColumn id="9" uniqueName="Category" name="Category" queryTableFieldId="8" dataDxfId="12"/>
     <tableColumn id="10" uniqueName="Probability" name="Probability of Occurrence (%) " queryTableFieldId="9" dataDxfId="11" dataCellStyle="Percent"/>
     <tableColumn id="11" uniqueName="Impact" name="Impact  _x000a_Rating   (1-5)" queryTableFieldId="10" dataDxfId="10" dataCellStyle="Currency"/>
-    <tableColumn id="21" uniqueName="21" name="Total Impact on occurance_x000a_$" queryTableFieldId="26" dataDxfId="9" dataCellStyle="Currency"/>
+    <tableColumn id="21" uniqueName="21" name="Total Impact on occurrence_x000a_$" queryTableFieldId="26" dataDxfId="9" dataCellStyle="Currency"/>
     <tableColumn id="12" uniqueName="Risk_x005f_x0020_Exposure" name="Risk Exposure Ranking_x000a_(1 - 25)" queryTableFieldId="11" dataDxfId="8"/>
     <tableColumn id="13" uniqueName="13" name="Risk Exposure Estimate   ($)" queryTableFieldId="24" dataDxfId="7">
-      <calculatedColumnFormula>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+      <calculatedColumnFormula>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="20" uniqueName="20" name="Basis of Risk Exposure Estimate" queryTableFieldId="25" dataDxfId="6"/>
@@ -1533,8 +1563,8 @@
   </sheetPr>
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,7 +1620,7 @@
     </row>
     <row r="2" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -1628,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>2</v>
@@ -1652,10 +1682,10 @@
         <v>18</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>16</v>
@@ -1684,11 +1714,11 @@
     </row>
     <row r="4" spans="1:22" ht="113.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="7">
         <v>40721</v>
@@ -1697,19 +1727,19 @@
         <v>42060</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="18" t="s">
+      <c r="I4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="K4" s="22">
         <v>1</v>
@@ -1726,52 +1756,52 @@
         <v>25</v>
       </c>
       <c r="O4" s="10" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R4" s="7">
         <v>41731</v>
       </c>
       <c r="S4" s="7"/>
       <c r="T4" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V4" s="7"/>
     </row>
     <row r="5" spans="1:22" ht="66.599999999999994" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="7">
         <v>41013</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="K5" s="22">
         <v>1</v>
@@ -1788,50 +1818,52 @@
         <v>5</v>
       </c>
       <c r="O5" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U5" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V5" s="7"/>
     </row>
     <row r="6" spans="1:22" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="4" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D6" s="7">
         <v>41108</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7">
+        <v>42403</v>
+      </c>
       <c r="F6" s="5" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="K6" s="22">
         <v>1</v>
@@ -1848,33 +1880,33 @@
         <v>5</v>
       </c>
       <c r="O6" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
       <c r="P6" s="12"/>
       <c r="Q6" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R6" s="7">
         <v>41731</v>
       </c>
       <c r="S6" s="7"/>
       <c r="T6" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="V6" s="7"/>
     </row>
     <row r="7" spans="1:22" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D7" s="9">
         <v>41414</v>
@@ -1883,19 +1915,19 @@
         <v>42058</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="K7" s="22">
         <v>1</v>
@@ -1912,33 +1944,33 @@
         <v>25</v>
       </c>
       <c r="O7" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
       <c r="P7" s="13"/>
       <c r="Q7" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R7" s="9">
         <v>41760</v>
       </c>
       <c r="S7" s="9"/>
       <c r="T7" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="V7" s="9"/>
     </row>
     <row r="8" spans="1:22" ht="66" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" s="9">
         <v>41438</v>
@@ -1947,19 +1979,19 @@
         <v>42060</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="K8" s="22">
         <v>1</v>
@@ -1976,33 +2008,33 @@
         <v>10</v>
       </c>
       <c r="O8" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R8" s="9">
         <v>41791</v>
       </c>
       <c r="S8" s="9"/>
       <c r="T8" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="U8" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="V8" s="9"/>
     </row>
     <row r="9" spans="1:22" ht="88.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D9" s="9">
         <v>41619</v>
@@ -2011,19 +2043,19 @@
         <v>41850</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="J9" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="K9" s="22">
         <v>0.25</v>
@@ -2040,13 +2072,13 @@
         <v>5</v>
       </c>
       <c r="O9" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
       <c r="P9" s="15"/>
       <c r="Q9" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R9" s="9">
         <v>41803</v>
@@ -2055,20 +2087,20 @@
         <v>41850</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="V9" s="9"/>
     </row>
     <row r="10" spans="1:22" ht="57.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D10" s="9">
         <v>41837</v>
@@ -2077,17 +2109,17 @@
         <v>42058</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K10" s="22">
         <v>0.75</v>
@@ -2104,7 +2136,7 @@
         <v>18.75</v>
       </c>
       <c r="O10" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2114,38 +2146,38 @@
       <c r="S10" s="9"/>
       <c r="T10" s="5"/>
       <c r="U10" s="4" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="V10" s="9"/>
     </row>
     <row r="11" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D11" s="9">
         <v>41850</v>
       </c>
       <c r="E11" s="9">
-        <v>42088</v>
+        <v>42403</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K11" s="22">
         <v>0.85</v>
@@ -2162,31 +2194,33 @@
         <v>21.25</v>
       </c>
       <c r="O11" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
       <c r="P11" s="15"/>
       <c r="Q11" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="R11" s="9">
         <v>41850</v>
       </c>
       <c r="S11" s="9"/>
       <c r="T11" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="U11" s="8"/>
+        <v>91</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="V11" s="9"/>
     </row>
-    <row r="12" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D12" s="9">
         <v>42060</v>
@@ -2195,19 +2229,19 @@
         <v>42137</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K12" s="22">
         <v>0.2</v>
@@ -2224,33 +2258,33 @@
         <v>3.0000000000000004</v>
       </c>
       <c r="O12" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
       <c r="P12" s="15"/>
       <c r="Q12" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="R12" s="9">
         <v>42064</v>
       </c>
       <c r="S12" s="9"/>
       <c r="T12" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="U12" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="V12" s="9"/>
     </row>
     <row r="13" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D13" s="9">
         <v>42137</v>
@@ -2259,19 +2293,19 @@
         <v>42270</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K13" s="22">
         <v>0.2</v>
@@ -2288,52 +2322,54 @@
         <v>3.0000000000000004</v>
       </c>
       <c r="O13" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
       <c r="P13" s="15"/>
       <c r="Q13" s="5" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="R13" s="9">
         <v>42142</v>
       </c>
       <c r="S13" s="9"/>
       <c r="T13" s="5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="U13" s="8" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="V13" s="9"/>
     </row>
     <row r="14" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D14" s="9">
         <v>42137</v>
       </c>
-      <c r="E14" s="9"/>
+      <c r="E14" s="9">
+        <v>42403</v>
+      </c>
       <c r="F14" s="5" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K14" s="22">
         <v>0.2</v>
@@ -2350,102 +2386,148 @@
         <v>3.0000000000000004</v>
       </c>
       <c r="O14" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
       <c r="P14" s="15"/>
       <c r="Q14" s="5" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="R14" s="9">
         <v>42142</v>
       </c>
       <c r="S14" s="9"/>
       <c r="T14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="U14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="V14" s="9"/>
+    </row>
+    <row r="15" spans="1:22" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="U14" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="V14" s="9"/>
-    </row>
-    <row r="15" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="9">
+        <v>42038</v>
+      </c>
       <c r="E15" s="9"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="19" t="s">
-        <v>20</v>
+      <c r="F15" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="L15" s="19">
+        <v>1</v>
       </c>
       <c r="M15" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="20" t="e">
+      <c r="N15" s="20">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
 Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="O15" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
       <c r="P15" s="15"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="9"/>
+      <c r="Q15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="R15" s="9">
+        <v>42403</v>
+      </c>
       <c r="S15" s="9"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="8"/>
+      <c r="T15" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="V15" s="9"/>
     </row>
-    <row r="16" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+    <row r="16" spans="1:22" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="B16" s="8"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="9"/>
+      <c r="C16" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="9">
+        <v>42403</v>
+      </c>
       <c r="E16" s="9"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" s="19" t="s">
-        <v>20</v>
+      <c r="F16" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="L16" s="19">
+        <v>4</v>
       </c>
       <c r="M16" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="20" t="e">
+      <c r="N16" s="20">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
 Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
+        <v>4</v>
       </c>
       <c r="O16" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
       <c r="P16" s="15"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="9"/>
+      <c r="Q16" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="R16" s="9">
+        <v>42403</v>
+      </c>
       <c r="S16" s="9"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="8"/>
+      <c r="T16" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="V16" s="9"/>
     </row>
     <row r="17" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -2474,7 +2556,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O17" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2512,7 +2594,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O18" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2550,7 +2632,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O19" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2588,7 +2670,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O20" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2626,7 +2708,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O21" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2664,7 +2746,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O22" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2702,7 +2784,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O23" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2740,7 +2822,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O24" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2778,7 +2860,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O25" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2816,7 +2898,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O26" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2854,7 +2936,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O27" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2892,7 +2974,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O28" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2930,7 +3012,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O29" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -2968,7 +3050,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O30" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -3006,7 +3088,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O31" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -3044,7 +3126,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O32" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -3082,7 +3164,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O33" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -3120,7 +3202,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O34" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -3158,7 +3240,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O35" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -3196,7 +3278,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O36" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -3234,7 +3316,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="O37" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurrence
 $]]</f>
         <v>#VALUE!</v>
       </c>
@@ -3252,7 +3334,7 @@
     <mergeCell ref="A2:V2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="17" scale="36" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="17" scale="59" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;LVangent Proprietary Information</oddFooter>
   </headerFooter>
@@ -3264,10 +3346,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3280,7 +3362,7 @@
         <v>42060</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3288,7 +3370,7 @@
         <v>42088</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3296,7 +3378,7 @@
         <v>42096</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3304,7 +3386,7 @@
         <v>42137</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3312,7 +3394,15 @@
         <v>42270</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>42403</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3327,15 +3417,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E5C6E04F5F2CA4DBF07DC2DA055DA5A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b67af60ff7fc8b8e5184fdb460baaf96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -3449,6 +3530,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
   <ds:schemaRefs>
@@ -3465,14 +3555,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9FB9A1-B4D8-4EF0-9C41-8E101BF6B1F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3486,4 +3568,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>